<commit_message>
nueva versión hasta relacion pruebas cliente
</commit_message>
<xml_diff>
--- a/STE/war/datadocs/templatePruebas.xlsx
+++ b/STE/war/datadocs/templatePruebas.xlsx
@@ -4,16 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17850" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17850" windowHeight="10320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DatosGraf" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="Clientes">Pruebas!$E$21</definedName>
     <definedName name="Estados">Pruebas!$F$9</definedName>
+    <definedName name="Resultados">DatosGraf!$C$18</definedName>
     <definedName name="Total">Pruebas!$I$9</definedName>
+    <definedName name="TotalPorCliente">Pruebas!$E$21</definedName>
+    <definedName name="TotalResultados">DatosGraf!$C$18</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -146,7 +150,70 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES_tradnl"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Pruebas por cliente</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[0]!Clientes</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[0]!TotalPorCliente</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -256,6 +323,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -551,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C8:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -639,7 +736,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
nuevos informes y cambios alcance
</commit_message>
<xml_diff>
--- a/STE/war/datadocs/templatePruebas.xlsx
+++ b/STE/war/datadocs/templatePruebas.xlsx
@@ -4,27 +4,29 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17850" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17850" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas" sheetId="1" r:id="rId1"/>
-    <sheet name="DatosGraf" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Clientes">Pruebas!$E$21</definedName>
+    <definedName name="Entorno">Pruebas!$G$63:$H$63</definedName>
     <definedName name="Estados">Pruebas!$F$9</definedName>
-    <definedName name="Resultados">DatosGraf!$C$18</definedName>
+    <definedName name="PruebasPorEntorno">Pruebas!$H$64:$I$64</definedName>
+    <definedName name="PruebasPorFichero">Pruebas!$G$30:$G$35</definedName>
+    <definedName name="Resultados">Pruebas!$F$30:$F$32</definedName>
+    <definedName name="TipoFichero">Pruebas!$F$30:$F$35</definedName>
     <definedName name="Total">Pruebas!$I$9</definedName>
     <definedName name="TotalPorCliente">Pruebas!$E$21</definedName>
-    <definedName name="TotalResultados">DatosGraf!$C$18</definedName>
+    <definedName name="TotalResultados">Pruebas!$G$30:$G$32</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>PRODUCCIÓN</t>
   </si>
@@ -32,10 +34,28 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>TOTAL PRUEBAS</t>
+    <t>INTEGRADO</t>
   </si>
   <si>
-    <t>INTEGRADO</t>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>Cancelada</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Número de Pruebas</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Total pruebas</t>
   </si>
 </sst>
 </file>
@@ -59,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -77,6 +97,45 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -86,10 +145,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -103,6 +165,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-ES_tradnl"/>
   <c:chart>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -110,6 +173,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Pruebas por estado</c:v>
+          </c:tx>
           <c:cat>
             <c:numRef>
               <c:f>[0]!Estados</c:f>
@@ -134,7 +200,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -150,7 +215,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -164,7 +229,17 @@
       <c:layout/>
     </c:title>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1010283550621786E-2"/>
+          <c:y val="0.18043999708369796"/>
+          <c:w val="0.45284711286089241"/>
+          <c:h val="0.75474518810148794"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -213,7 +288,235 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES_tradnl"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29164654418197727"/>
+          <c:y val="0.18969925634295728"/>
+          <c:w val="0.45284711286089241"/>
+          <c:h val="0.75474518810148794"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Pruebas por resultado</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>[0]!Resultados</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>OK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cancelada</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[0]!TotalResultados</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES_tradnl"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22687204724409449"/>
+          <c:y val="0.17435922585801344"/>
+          <c:w val="0.45701377952755912"/>
+          <c:h val="0.75643660059733908"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Pruebas por fichero</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>[0]!TipoFichero</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>OK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cancelada</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[0]!PruebasPorFichero</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES_tradnl"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Pruebas por entorno</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>[0]!Entorno</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[0]!PruebasPorEntorno</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -330,16 +633,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -353,6 +656,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -646,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C8:I25"/>
+  <dimension ref="F8:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,102 +1051,105 @@
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
     <col min="13" max="13" width="8.140625" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="6:9">
-      <c r="G8" s="1" t="s">
+    <row r="8" spans="6:9" ht="15.75" thickBot="1">
+      <c r="F8" s="3"/>
+      <c r="G8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="6:9">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="6:9">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="6:9">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="6:9">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="6:9">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="6:9">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="29" spans="6:8" ht="15.75" thickBot="1">
+      <c r="F29" s="3"/>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="6:8">
+      <c r="F30" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>0</v>
+    </row>
+    <row r="31" spans="6:8">
+      <c r="F31" s="4" t="s">
+        <v>4</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>1</v>
+    </row>
+    <row r="32" spans="6:8" ht="15.75" thickBot="1">
+      <c r="F32" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="9" spans="6:9">
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="6:9">
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="6:9">
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="6:9">
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="6:9">
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="6:9">
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="25" spans="3:5">
-      <c r="C25" s="1" t="s">
-        <v>3</v>
+    <row r="33" spans="6:6">
+      <c r="F33" s="5" t="s">
+        <v>6</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>0</v>
+    </row>
+    <row r="49" spans="6:8" ht="15.75" thickBot="1">
+      <c r="F49" s="3"/>
+      <c r="G49" s="2" t="s">
+        <v>9</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>2</v>
+      <c r="H49" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cambios de alcance corregidos
</commit_message>
<xml_diff>
--- a/STE/war/datadocs/templatePruebas.xlsx
+++ b/STE/war/datadocs/templatePruebas.xlsx
@@ -215,7 +215,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -234,10 +234,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.1010283550621786E-2"/>
-          <c:y val="0.18043999708369796"/>
+          <c:x val="4.1010283550621807E-2"/>
+          <c:y val="0.18043999708369798"/>
           <c:w val="0.45284711286089241"/>
-          <c:h val="0.75474518810148794"/>
+          <c:h val="0.75474518810148805"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -288,7 +288,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -308,9 +308,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.29164654418197727"/>
-          <c:y val="0.18969925634295728"/>
+          <c:y val="0.18969925634295731"/>
           <c:w val="0.45284711286089241"/>
-          <c:h val="0.75474518810148794"/>
+          <c:h val="0.75474518810148805"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -369,7 +369,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -388,9 +388,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22687204724409449"/>
+          <c:x val="0.11377099737532809"/>
           <c:y val="0.17435922585801344"/>
-          <c:w val="0.45701377952755912"/>
+          <c:w val="0.45701377952755917"/>
           <c:h val="0.75643660059733908"/>
         </c:manualLayout>
       </c:layout>
@@ -453,7 +453,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -516,7 +516,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1041,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F8:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>

</xml_diff>